<commit_message>
Update: Improve setting of area_id
</commit_message>
<xml_diff>
--- a/inst/input.xlsx
+++ b/inst/input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="217">
   <si>
     <t>牛舎間の移動の設定</t>
     <rPh sb="0" eb="2">
@@ -1958,6 +1958,44 @@
     </rPh>
     <rPh sb="65" eb="66">
       <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※新生子牛用牛舎</t>
+    <rPh sb="1" eb="3">
+      <t>アラオイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウシ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ギュウシャ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※一行目は必ず新生子牛用の牛舎にすること</t>
+    <rPh sb="1" eb="4">
+      <t>イチギョウメ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シンセイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>コウシ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ギュウシャ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -2051,7 +2089,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2160,13 +2198,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2324,6 +2375,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2801,11 +2861,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2813,6 +2873,7 @@
     <col min="1" max="1" width="9" style="11"/>
     <col min="2" max="2" width="16.625" style="11" customWidth="1"/>
     <col min="3" max="3" width="11.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2857,6 +2918,11 @@
       </c>
       <c r="C4" s="29" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="53" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3971,189 +4037,213 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7.875" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:7" ht="27">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C5" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="D5" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="G5" s="32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="18" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="31" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="G9" s="32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="13" t="s">
+    <row r="10" spans="1:7">
+      <c r="F10" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="E9" s="13"/>
-      <c r="F9" s="16" t="s">
+    <row r="11" spans="1:7">
+      <c r="F11" s="13"/>
+      <c r="G11" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="E10" s="13"/>
-      <c r="F10" s="16" t="s">
+    <row r="12" spans="1:7">
+      <c r="F12" s="13"/>
+      <c r="G12" s="16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11" s="13"/>
-      <c r="F11" s="16" t="s">
+    <row r="13" spans="1:7">
+      <c r="F13" s="13"/>
+      <c r="G13" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="E12" s="13"/>
-      <c r="F12" s="16" t="s">
+    <row r="14" spans="1:7">
+      <c r="F14" s="13"/>
+      <c r="G14" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="E13" s="17"/>
-      <c r="F13" s="19" t="s">
+    <row r="15" spans="1:7">
+      <c r="F15" s="17"/>
+      <c r="G15" s="19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="E14" s="36" t="s">
+    <row r="16" spans="1:7">
+      <c r="F16" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="G16" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15" s="13" t="s">
+    <row r="17" spans="6:7">
+      <c r="F17" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="G17" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="E16" s="13"/>
-      <c r="F16" s="16" t="s">
+    <row r="18" spans="6:7">
+      <c r="F18" s="13"/>
+      <c r="G18" s="16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="5:6">
-      <c r="E17" s="13"/>
-      <c r="F17" s="16" t="s">
+    <row r="19" spans="6:7">
+      <c r="F19" s="13"/>
+      <c r="G19" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="5:6">
-      <c r="E18" s="13"/>
-      <c r="F18" s="16" t="s">
+    <row r="20" spans="6:7">
+      <c r="F20" s="13"/>
+      <c r="G20" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="5:6">
-      <c r="E19" s="17"/>
-      <c r="F19" s="23" t="s">
+    <row r="21" spans="6:7">
+      <c r="F21" s="17"/>
+      <c r="G21" s="23" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean: Unselect cells in input.xlsx
</commit_message>
<xml_diff>
--- a/inst/input.xlsx
+++ b/inst/input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="214">
   <si>
     <t>牛舎間の移動の設定</t>
     <rPh sb="0" eb="2">
@@ -951,10 +951,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ハッチ</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1028,10 +1024,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>搾乳</t>
     <rPh sb="0" eb="2">
       <t>サク</t>
@@ -1056,10 +1048,6 @@
   </si>
   <si>
     <t>milking</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>s</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -2865,7 +2853,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2922,7 +2910,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="53" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3215,11 +3203,8 @@
       <c r="F5" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="N5" s="11">
         <v>1</v>
@@ -3243,22 +3228,22 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="N6" s="11">
         <v>5</v>
       </c>
       <c r="R6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3273,20 +3258,17 @@
         <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N7" s="11">
         <v>8</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3301,10 +3283,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>81</v>
@@ -3313,10 +3292,10 @@
         <v>13</v>
       </c>
       <c r="R8" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="S8" s="37" t="s">
         <v>127</v>
-      </c>
-      <c r="S8" s="37" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3331,13 +3310,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="N9" s="11">
         <v>1</v>
@@ -3346,10 +3322,10 @@
         <v>1</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -3364,13 +3340,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N10" s="11">
         <v>7</v>
@@ -3382,10 +3355,10 @@
         <v>1</v>
       </c>
       <c r="R10" s="46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -3400,13 +3373,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I11" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="N11" s="11">
         <v>3</v>
@@ -3415,7 +3385,7 @@
         <v>74</v>
       </c>
       <c r="S11" s="49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -3429,13 +3399,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N12" s="11">
         <v>2</v>
@@ -3445,7 +3412,7 @@
       </c>
       <c r="R12" s="50"/>
       <c r="S12" s="51" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -3459,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
@@ -3468,19 +3435,19 @@
         <v>2</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J13" s="52">
         <v>41919</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N13" s="11">
         <v>4</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="S13" s="21" t="s">
         <v>2</v>
@@ -3497,13 +3464,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N14" s="11">
         <v>3</v>
@@ -3512,31 +3476,31 @@
         <v>74</v>
       </c>
       <c r="S14" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="R15" s="13"/>
       <c r="S15" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="R16" s="13"/>
       <c r="S16" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="18:19">
       <c r="R17" s="13"/>
       <c r="S17" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="18:19">
       <c r="R18" s="17"/>
       <c r="S18" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="18:19">
@@ -3549,46 +3513,46 @@
     </row>
     <row r="20" spans="18:19">
       <c r="R20" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="18:19">
       <c r="R21" s="13"/>
       <c r="S21" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="18:19">
       <c r="R22" s="13"/>
       <c r="S22" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="18:19">
       <c r="R23" s="13"/>
       <c r="S23" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="18:19">
       <c r="R24" s="13"/>
       <c r="S24" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="18:19">
       <c r="R25" s="13"/>
       <c r="S25" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="18:19">
       <c r="R26" s="17"/>
       <c r="S26" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="18:19">
@@ -3604,36 +3568,36 @@
         <v>74</v>
       </c>
       <c r="S28" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="18:19">
       <c r="R29" s="13"/>
       <c r="S29" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="18:19">
       <c r="R30" s="13"/>
       <c r="S30" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="18:19">
       <c r="R31" s="13"/>
       <c r="S31" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="18:19">
       <c r="R32" s="17"/>
       <c r="S32" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="18:19">
       <c r="R33" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>2</v>
@@ -3641,21 +3605,21 @@
     </row>
     <row r="34" spans="18:19">
       <c r="R34" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S34" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="18:19">
       <c r="R35" s="17"/>
       <c r="S35" s="19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="18:19">
       <c r="R36" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>2</v>
@@ -3663,27 +3627,27 @@
     </row>
     <row r="37" spans="18:19">
       <c r="R37" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="18:19">
       <c r="R38" s="13"/>
       <c r="S38" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="18:19">
       <c r="R39" s="17"/>
       <c r="S39" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="18:19">
       <c r="R40" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>2</v>
@@ -3691,21 +3655,21 @@
     </row>
     <row r="41" spans="18:19">
       <c r="R41" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="18:19">
       <c r="R42" s="17"/>
       <c r="S42" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="18:19">
       <c r="R43" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>2</v>
@@ -3716,13 +3680,13 @@
         <v>74</v>
       </c>
       <c r="S44" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="18:19">
       <c r="R45" s="17"/>
       <c r="S45" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="18:19">
@@ -3735,33 +3699,33 @@
     </row>
     <row r="47" spans="18:19">
       <c r="R47" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="18:19">
       <c r="R48" s="13"/>
       <c r="S48" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="18:19">
       <c r="R49" s="13"/>
       <c r="S49" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="18:19">
       <c r="R50" s="17"/>
       <c r="S50" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="18:19">
       <c r="R51" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>2</v>
@@ -3769,22 +3733,22 @@
     </row>
     <row r="52" spans="18:19">
       <c r="R52" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="18:19">
       <c r="R53" s="13"/>
       <c r="S53" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="18:19">
       <c r="R54" s="17"/>
       <c r="S54" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="18:19">
@@ -3797,45 +3761,45 @@
     </row>
     <row r="56" spans="18:19">
       <c r="R56" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="18:19">
       <c r="R57" s="13"/>
       <c r="S57" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="18:19">
       <c r="R58" s="13"/>
       <c r="S58" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="18:19">
       <c r="R59" s="13"/>
       <c r="S59" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="18:19">
       <c r="R60" s="13"/>
       <c r="S60" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="18:19">
       <c r="R61" s="17"/>
       <c r="S61" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="18:19">
       <c r="R62" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S62" s="21" t="s">
         <v>2</v>
@@ -3846,19 +3810,19 @@
         <v>74</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="18:19">
       <c r="R64" s="13"/>
       <c r="S64" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="18:19">
       <c r="R65" s="17"/>
       <c r="S65" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="18:19">
@@ -3874,13 +3838,13 @@
         <v>74</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="18:19">
       <c r="R68" s="17"/>
       <c r="S68" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="18:19">
@@ -3893,21 +3857,21 @@
     </row>
     <row r="70" spans="18:19">
       <c r="R70" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="18:19">
       <c r="R71" s="17"/>
       <c r="S71" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="18:19">
       <c r="R72" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S72" s="21" t="s">
         <v>2</v>
@@ -3918,19 +3882,19 @@
         <v>74</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="18:19">
       <c r="R74" s="13"/>
       <c r="S74" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="18:19">
       <c r="R75" s="13"/>
       <c r="S75" s="16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="18:19">
@@ -3943,10 +3907,10 @@
     </row>
     <row r="77" spans="18:19">
       <c r="R77" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S77" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="18:19">
@@ -3959,28 +3923,28 @@
     </row>
     <row r="79" spans="18:19">
       <c r="R79" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="18:19">
       <c r="R80" s="13"/>
       <c r="S80" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="18:19">
       <c r="R81" s="13"/>
       <c r="S81" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="18:19">
       <c r="R82" s="17"/>
       <c r="S82" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="18:19">
@@ -3993,40 +3957,40 @@
     </row>
     <row r="84" spans="18:19">
       <c r="R84" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="S84" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="18:19">
       <c r="R85" s="13"/>
       <c r="S85" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="18:19">
       <c r="R86" s="13"/>
       <c r="S86" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="18:19">
       <c r="R87" s="13"/>
       <c r="S87" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="18:19">
       <c r="R88" s="13"/>
       <c r="S88" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" spans="18:19">
       <c r="R89" s="17"/>
       <c r="S89" s="19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4105,7 +4069,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>65</v>
@@ -4137,7 +4101,7 @@
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="55" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4152,7 +4116,7 @@
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4364,7 +4328,7 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4522,7 +4486,7 @@
     <row r="25" spans="6:7">
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="6:7">
@@ -4544,7 +4508,7 @@
     <row r="28" spans="6:7">
       <c r="F28" s="13"/>
       <c r="G28" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="6:7">

</xml_diff>

<commit_message>
Rename `communal pasture` to `pasture`
</commit_message>
<xml_diff>
--- a/inst/input.xlsx
+++ b/inst/input.xlsx
@@ -678,10 +678,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>communal pasture</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>牛舎の種類</t>
     <rPh sb="0" eb="2">
       <t>ギュウシャ</t>
@@ -692,14 +688,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>hatch: ハッチ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>free: フリーストール・フリーバーン</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>outside: 放牧・パドック</t>
     <rPh sb="9" eb="11">
       <t>ホウボク</t>
@@ -713,19 +701,6 @@
     </rPh>
     <rPh sb="7" eb="8">
       <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>communal pasture: 預託牧場・公共牧場</t>
-    <rPh sb="18" eb="20">
-      <t>ヨタク</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ボクジョウ</t>
-    </rPh>
-    <rPh sb="23" eb="27">
-      <t>コウキョウ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -1985,6 +1960,31 @@
     <rPh sb="13" eb="15">
       <t>ギュウシャ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>pasture: 預託牧場・公共牧場</t>
+    <rPh sb="9" eb="11">
+      <t>ヨタク</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ボクジョウ</t>
+    </rPh>
+    <rPh sb="14" eb="18">
+      <t>コウキョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>pasture</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hatch: ハッチ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>free: フリーストール・フリーバーン・ペン</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2704,7 +2704,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2745,10 +2745,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>2</v>
@@ -2772,72 +2772,72 @@
         <v>2</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="F4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="G4" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="53" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3018,7 +3018,7 @@
   <dimension ref="A1:S89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
@@ -3047,7 +3047,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3088,10 +3088,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>2</v>
@@ -3115,72 +3115,72 @@
         <v>2</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M3" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N3" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="P3" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="F4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="G4" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="R4" s="7" t="s">
         <v>68</v>
@@ -3195,22 +3195,22 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E5" s="11">
         <v>0</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="N5" s="11">
         <v>1</v>
       </c>
       <c r="R5" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S5" s="21" t="s">
         <v>2</v>
@@ -3228,22 +3228,22 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N6" s="11">
         <v>5</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3258,17 +3258,17 @@
         <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N7" s="11">
         <v>8</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3283,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>81</v>
@@ -3292,10 +3292,10 @@
         <v>13</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S8" s="37" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3310,10 +3310,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N9" s="11">
         <v>1</v>
@@ -3322,10 +3322,10 @@
         <v>1</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -3340,10 +3340,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N10" s="11">
         <v>7</v>
@@ -3355,10 +3355,10 @@
         <v>1</v>
       </c>
       <c r="R10" s="46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -3373,10 +3373,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N11" s="11">
         <v>3</v>
@@ -3385,7 +3385,7 @@
         <v>74</v>
       </c>
       <c r="S11" s="49" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -3399,10 +3399,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N12" s="11">
         <v>2</v>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="R12" s="50"/>
       <c r="S12" s="51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -3426,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
@@ -3435,19 +3435,19 @@
         <v>2</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J13" s="52">
         <v>41919</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N13" s="11">
         <v>4</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="S13" s="21" t="s">
         <v>2</v>
@@ -3464,10 +3464,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N14" s="11">
         <v>3</v>
@@ -3476,36 +3476,36 @@
         <v>74</v>
       </c>
       <c r="S14" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="R15" s="13"/>
       <c r="S15" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="R16" s="13"/>
       <c r="S16" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="18:19">
       <c r="R17" s="13"/>
       <c r="S17" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="18:19">
       <c r="R18" s="17"/>
       <c r="S18" s="19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="18:19">
       <c r="R19" s="20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>2</v>
@@ -3513,51 +3513,51 @@
     </row>
     <row r="20" spans="18:19">
       <c r="R20" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="18:19">
       <c r="R21" s="13"/>
       <c r="S21" s="16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="18:19">
       <c r="R22" s="13"/>
       <c r="S22" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="18:19">
       <c r="R23" s="13"/>
       <c r="S23" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="18:19">
       <c r="R24" s="13"/>
       <c r="S24" s="16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="18:19">
       <c r="R25" s="13"/>
       <c r="S25" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="18:19">
       <c r="R26" s="17"/>
       <c r="S26" s="19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="18:19">
       <c r="R27" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="S27" s="21" t="s">
         <v>2</v>
@@ -3568,36 +3568,36 @@
         <v>74</v>
       </c>
       <c r="S28" s="16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="18:19">
       <c r="R29" s="13"/>
       <c r="S29" s="16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="18:19">
       <c r="R30" s="13"/>
       <c r="S30" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="18:19">
       <c r="R31" s="13"/>
       <c r="S31" s="16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="18:19">
       <c r="R32" s="17"/>
       <c r="S32" s="19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="18:19">
       <c r="R33" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>2</v>
@@ -3605,21 +3605,21 @@
     </row>
     <row r="34" spans="18:19">
       <c r="R34" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S34" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="18:19">
       <c r="R35" s="17"/>
       <c r="S35" s="19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="18:19">
       <c r="R36" s="20" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>2</v>
@@ -3627,27 +3627,27 @@
     </row>
     <row r="37" spans="18:19">
       <c r="R37" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="18:19">
       <c r="R38" s="13"/>
       <c r="S38" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="18:19">
       <c r="R39" s="17"/>
       <c r="S39" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="18:19">
       <c r="R40" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>2</v>
@@ -3655,21 +3655,21 @@
     </row>
     <row r="41" spans="18:19">
       <c r="R41" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="S41" s="16" t="s">
         <v>165</v>
-      </c>
-      <c r="S41" s="16" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="42" spans="18:19">
       <c r="R42" s="17"/>
       <c r="S42" s="19" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="18:19">
       <c r="R43" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>2</v>
@@ -3680,18 +3680,18 @@
         <v>74</v>
       </c>
       <c r="S44" s="16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="18:19">
       <c r="R45" s="17"/>
       <c r="S45" s="19" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="18:19">
       <c r="R46" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="S46" s="21" t="s">
         <v>2</v>
@@ -3699,33 +3699,33 @@
     </row>
     <row r="47" spans="18:19">
       <c r="R47" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="18:19">
       <c r="R48" s="13"/>
       <c r="S48" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="18:19">
       <c r="R49" s="13"/>
       <c r="S49" s="16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="18:19">
       <c r="R50" s="17"/>
       <c r="S50" s="19" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="18:19">
       <c r="R51" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>2</v>
@@ -3733,27 +3733,27 @@
     </row>
     <row r="52" spans="18:19">
       <c r="R52" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="18:19">
       <c r="R53" s="13"/>
       <c r="S53" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="18:19">
       <c r="R54" s="17"/>
       <c r="S54" s="19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="18:19">
       <c r="R55" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S55" s="21" t="s">
         <v>2</v>
@@ -3761,45 +3761,45 @@
     </row>
     <row r="56" spans="18:19">
       <c r="R56" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="18:19">
       <c r="R57" s="13"/>
       <c r="S57" s="16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="18:19">
       <c r="R58" s="13"/>
       <c r="S58" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="18:19">
       <c r="R59" s="13"/>
       <c r="S59" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="18:19">
       <c r="R60" s="13"/>
       <c r="S60" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="18:19">
       <c r="R61" s="17"/>
       <c r="S61" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="18:19">
       <c r="R62" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="S62" s="21" t="s">
         <v>2</v>
@@ -3810,24 +3810,24 @@
         <v>74</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="18:19">
       <c r="R64" s="13"/>
       <c r="S64" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="18:19">
       <c r="R65" s="17"/>
       <c r="S65" s="19" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="18:19">
       <c r="R66" s="20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S66" s="21" t="s">
         <v>2</v>
@@ -3838,18 +3838,18 @@
         <v>74</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="18:19">
       <c r="R68" s="17"/>
       <c r="S68" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="18:19">
       <c r="R69" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S69" s="21" t="s">
         <v>2</v>
@@ -3857,21 +3857,21 @@
     </row>
     <row r="70" spans="18:19">
       <c r="R70" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="18:19">
       <c r="R71" s="17"/>
       <c r="S71" s="19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="18:19">
       <c r="R72" s="20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S72" s="21" t="s">
         <v>2</v>
@@ -3882,24 +3882,24 @@
         <v>74</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="18:19">
       <c r="R74" s="13"/>
       <c r="S74" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="18:19">
       <c r="R75" s="13"/>
       <c r="S75" s="16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="18:19">
       <c r="R76" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="S76" s="21" t="s">
         <v>2</v>
@@ -3907,15 +3907,15 @@
     </row>
     <row r="77" spans="18:19">
       <c r="R77" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S77" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="18:19">
       <c r="R78" s="20" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="S78" s="21" t="s">
         <v>2</v>
@@ -3923,33 +3923,33 @@
     </row>
     <row r="79" spans="18:19">
       <c r="R79" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="18:19">
       <c r="R80" s="13"/>
       <c r="S80" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="18:19">
       <c r="R81" s="13"/>
       <c r="S81" s="16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="18:19">
       <c r="R82" s="17"/>
       <c r="S82" s="19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="18:19">
       <c r="R83" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="S83" s="21" t="s">
         <v>2</v>
@@ -3957,40 +3957,40 @@
     </row>
     <row r="84" spans="18:19">
       <c r="R84" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="S84" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="18:19">
       <c r="R85" s="13"/>
       <c r="S85" s="16" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="18:19">
       <c r="R86" s="13"/>
       <c r="S86" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="18:19">
       <c r="R87" s="13"/>
       <c r="S87" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="18:19">
       <c r="R88" s="13"/>
       <c r="S88" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="18:19">
       <c r="R89" s="17"/>
       <c r="S89" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4069,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>65</v>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="55" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4124,7 +4124,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>80</v>
@@ -4138,45 +4138,45 @@
         <v>74</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="F11" s="13"/>
       <c r="G11" s="16" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="F12" s="13"/>
       <c r="G12" s="16" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="F13" s="13"/>
       <c r="G13" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="F14" s="13"/>
       <c r="G14" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="F15" s="17"/>
       <c r="G15" s="19" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="F16" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="6:7">
@@ -4184,31 +4184,31 @@
         <v>74</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="6:7">
       <c r="F18" s="13"/>
       <c r="G18" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="6:7">
       <c r="F19" s="13"/>
       <c r="G19" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="6:7">
       <c r="F20" s="13"/>
       <c r="G20" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="6:7">
       <c r="F21" s="17"/>
       <c r="G21" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -4328,7 +4328,7 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4486,7 +4486,7 @@
     <row r="25" spans="6:7">
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="6:7">
@@ -4508,7 +4508,7 @@
     <row r="28" spans="6:7">
       <c r="F28" s="13"/>
       <c r="G28" s="16" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="6:7">

</xml_diff>

<commit_message>
Fix typo in input.xlsx
</commit_message>
<xml_diff>
--- a/inst/input.xlsx
+++ b/inst/input.xlsx
@@ -1509,10 +1509,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>process_raw_area()またはprocess_raw_cow()のmodify_prevalenceに0-1の値を設定することで農場内のウイルス陽性率を設定することもできる</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>date_ial</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1985,6 +1981,10 @@
   </si>
   <si>
     <t>free: フリーストール・フリーバーン・ペン</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>prepare_data()またはprepare_cows()のmodify_prevalenceに0-1の値を設定することで農場内のウイルス陽性率を設定することもできる</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3018,7 +3018,7 @@
   <dimension ref="A1:S89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
@@ -3794,12 +3794,12 @@
     <row r="61" spans="18:19">
       <c r="R61" s="17"/>
       <c r="S61" s="19" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="18:19">
       <c r="R62" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S62" s="21" t="s">
         <v>2</v>
@@ -3810,7 +3810,7 @@
         <v>74</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="18:19">
@@ -3822,7 +3822,7 @@
     <row r="65" spans="18:19">
       <c r="R65" s="17"/>
       <c r="S65" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="18:19">
@@ -3838,13 +3838,13 @@
         <v>74</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="18:19">
       <c r="R68" s="17"/>
       <c r="S68" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="18:19">
@@ -3860,18 +3860,18 @@
         <v>168</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="18:19">
       <c r="R71" s="17"/>
       <c r="S71" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="18:19">
       <c r="R72" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S72" s="21" t="s">
         <v>2</v>
@@ -3882,19 +3882,19 @@
         <v>74</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="18:19">
       <c r="R74" s="13"/>
       <c r="S74" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="18:19">
       <c r="R75" s="13"/>
       <c r="S75" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="18:19">
@@ -3910,7 +3910,7 @@
         <v>119</v>
       </c>
       <c r="S77" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="18:19">
@@ -3926,25 +3926,25 @@
         <v>119</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="18:19">
       <c r="R80" s="13"/>
       <c r="S80" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="18:19">
       <c r="R81" s="13"/>
       <c r="S81" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="18:19">
       <c r="R82" s="17"/>
       <c r="S82" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="18:19">
@@ -3957,40 +3957,40 @@
     </row>
     <row r="84" spans="18:19">
       <c r="R84" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="S84" s="16" t="s">
         <v>197</v>
-      </c>
-      <c r="S84" s="16" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="85" spans="18:19">
       <c r="R85" s="13"/>
       <c r="S85" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="18:19">
       <c r="R86" s="13"/>
       <c r="S86" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" spans="18:19">
       <c r="R87" s="13"/>
       <c r="S87" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="18:19">
       <c r="R88" s="13"/>
       <c r="S88" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="18:19">
       <c r="R89" s="17"/>
       <c r="S89" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4069,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>65</v>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4124,7 +4124,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>80</v>
@@ -4144,13 +4144,13 @@
     <row r="11" spans="1:7">
       <c r="F11" s="13"/>
       <c r="G11" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="F12" s="13"/>
       <c r="G12" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4168,7 +4168,7 @@
     <row r="15" spans="1:7">
       <c r="F15" s="17"/>
       <c r="G15" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4486,7 +4486,7 @@
     <row r="25" spans="6:7">
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="6:7">
@@ -4508,7 +4508,7 @@
     <row r="28" spans="6:7">
       <c r="F28" s="13"/>
       <c r="G28" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="6:7">

</xml_diff>